<commit_message>
can parse expressions, not functions though
</commit_message>
<xml_diff>
--- a/test/simple_formula_testing.xlsx
+++ b/test/simple_formula_testing.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="another, sheet" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,26 +21,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t xml:space="preserve">values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">formulas</t>
+  </si>
   <si>
     <t xml:space="preserve">bird</t>
   </si>
   <si>
     <t xml:space="preserve">glass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">more values</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -99,8 +111,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -121,48 +145,83 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:C6"/>
+  <dimension ref="A2:C11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="C3" s="0" t="str">
+      <c r="C3" s="1" t="str">
         <f aca="false">"just a string"</f>
         <v>just a string</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="C4" s="0" t="str">
+      <c r="C4" s="1" t="str">
         <f aca="false">"string w "" quote"</f>
         <v>string w " quote</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="0" t="n">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="n">
         <f aca="false">A3+A4</f>
         <v>120</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="0" t="str">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="str">
         <f aca="false">A5&amp;A6</f>
         <v>birdglass</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="1" t="n">
+        <f aca="false">A3+'another, sheet'!A5</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="2" t="n">
+        <f aca="false">A3+A4*2</f>
+        <v>220</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="0" t="n">
+        <f aca="false">SUM(A3:A4)</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="3" t="b">
+        <f aca="false">AND(A4&gt;10,A3=20)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -174,4 +233,48 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A3:A6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>